<commit_message>
Updating data file names.
</commit_message>
<xml_diff>
--- a/data/female_conditioning/ovod1/4-1_1-4_oviposition_ovod1_b1.xlsx
+++ b/data/female_conditioning/ovod1/4-1_1-4_oviposition_ovod1_b1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster/data/female_conditioning/ovod1/block_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_4/data/female_conditioning/ovod1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97891B5E-08FF-574D-9CE6-12B3746D436A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6107E54C-5FBE-4745-A4D9-32DDF7CD745E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{AC32D7B1-1306-D046-90E4-7C831C04A1D9}"/>
+    <workbookView xWindow="220" yWindow="3920" windowWidth="28040" windowHeight="16100" xr2:uid="{AC32D7B1-1306-D046-90E4-7C831C04A1D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -146,7 +146,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -252,7 +252,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -394,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -404,16 +404,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6BCF0C-54AE-A547-83A4-3F41544B1E9A}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="A10:E12"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="4" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -421,16 +420,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -438,16 +437,16 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <v>28</v>
+      </c>
+      <c r="C2">
         <v>172</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
         <v>18</v>
-      </c>
-      <c r="D2">
-        <v>28</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -455,16 +454,16 @@
         <v>2</v>
       </c>
       <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
         <v>191</v>
       </c>
-      <c r="C3">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>5</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -472,16 +471,16 @@
         <v>3</v>
       </c>
       <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
         <v>226</v>
       </c>
-      <c r="C4">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>9</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -489,16 +488,16 @@
         <v>4</v>
       </c>
       <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
         <v>182</v>
       </c>
-      <c r="C5">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>24</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -506,16 +505,16 @@
         <v>5</v>
       </c>
       <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
         <v>225</v>
       </c>
-      <c r="C6">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>27</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -523,16 +522,16 @@
         <v>6</v>
       </c>
       <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
         <v>221</v>
       </c>
-      <c r="C7">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>27</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -540,16 +539,16 @@
         <v>7</v>
       </c>
       <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
         <v>102</v>
       </c>
-      <c r="C8">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>118</v>
-      </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -557,16 +556,16 @@
         <v>8</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>170</v>
       </c>
-      <c r="C9">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <v>44</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating a data file.
</commit_message>
<xml_diff>
--- a/data/female_conditioning/ovod1/4-1_1-4_oviposition_ovod1_b1.xlsx
+++ b/data/female_conditioning/ovod1/4-1_1-4_oviposition_ovod1_b1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_4/data/female_conditioning/ovod1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiemillar/Documents/drosophila_project_2024/data/female_conditioning/ovod1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6107E54C-5FBE-4745-A4D9-32DDF7CD745E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C2861B-1D00-8C46-939A-0BA92E3FA7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="3920" windowWidth="28040" windowHeight="16100" xr2:uid="{AC32D7B1-1306-D046-90E4-7C831C04A1D9}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{AC32D7B1-1306-D046-90E4-7C831C04A1D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,10 +57,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6BCF0C-54AE-A547-83A4-3F41544B1E9A}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="265" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,16 +529,16 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>12</v>
       </c>
       <c r="C7">
         <v>221</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>27</v>
       </c>
     </row>
@@ -566,6 +574,24 @@
       </c>
       <c r="E9">
         <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <f>SUM(B2:B9)/8</f>
+        <v>10.625</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:E10" si="0">SUM(C2:C9)/8</f>
+        <v>186.125</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.375</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>